<commit_message>
Removed an incorrect observation (OECD-SIGI-9_HTI_2012)
</commit_message>
<xml_diff>
--- a/Simple_XLS_Importer/data/OECD-SIGI/OECD-SIGI-9.xlsx
+++ b/Simple_XLS_Importer/data/OECD-SIGI/OECD-SIGI-9.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlos\Documents\projects\landbook-importers\Simple_XLS_Importer\data\OECD-SIGI\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="555" yWindow="555" windowWidth="20730" windowHeight="11760" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="552" yWindow="552" windowWidth="20736" windowHeight="11760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -21,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="291">
   <si>
     <t>country</t>
   </si>
@@ -240,9 +245,6 @@
     <t>Guinea-Bissau</t>
   </si>
   <si>
-    <t>Haiti</t>
-  </si>
-  <si>
     <t>Honduras</t>
   </si>
   <si>
@@ -934,9 +936,6 @@
   </si>
   <si>
     <t xml:space="preserve">  Zimbabwe</t>
-  </si>
-  <si>
-    <t>..</t>
   </si>
   <si>
     <t>SIGI-9</t>
@@ -945,8 +944,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1050,6 +1049,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1374,21 +1381,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C280"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C279"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A203" sqref="A203:XFD203"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49:XFD49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="10.875" style="2"/>
-    <col min="3" max="3" width="52.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.875" style="2"/>
+    <col min="1" max="2" width="10.8984375" style="2"/>
+    <col min="3" max="3" width="52.09765625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.8984375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1399,7 +1406,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>12</v>
       </c>
@@ -1410,7 +1417,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>13</v>
       </c>
@@ -1421,7 +1428,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>14</v>
       </c>
@@ -1432,7 +1439,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>15</v>
       </c>
@@ -1443,7 +1450,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>16</v>
       </c>
@@ -1454,7 +1461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>17</v>
       </c>
@@ -1465,7 +1472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>18</v>
       </c>
@@ -1476,7 +1483,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>19</v>
       </c>
@@ -1487,7 +1494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>20</v>
       </c>
@@ -1498,7 +1505,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>21</v>
       </c>
@@ -1509,7 +1516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>22</v>
       </c>
@@ -1520,7 +1527,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>23</v>
       </c>
@@ -1531,7 +1538,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>24</v>
       </c>
@@ -1542,7 +1549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>25</v>
       </c>
@@ -1553,7 +1560,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>26</v>
       </c>
@@ -1564,7 +1571,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>27</v>
       </c>
@@ -1575,7 +1582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>28</v>
       </c>
@@ -1586,7 +1593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>29</v>
       </c>
@@ -1597,7 +1604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
         <v>30</v>
       </c>
@@ -1608,7 +1615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>31</v>
       </c>
@@ -1619,7 +1626,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>32</v>
       </c>
@@ -1630,7 +1637,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>33</v>
       </c>
@@ -1641,7 +1648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>34</v>
       </c>
@@ -1652,7 +1659,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>35</v>
       </c>
@@ -1663,7 +1670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
         <v>36</v>
       </c>
@@ -1674,7 +1681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
         <v>37</v>
       </c>
@@ -1685,7 +1692,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
         <v>38</v>
       </c>
@@ -1696,7 +1703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
         <v>39</v>
       </c>
@@ -1707,7 +1714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
         <v>40</v>
       </c>
@@ -1718,7 +1725,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
         <v>41</v>
       </c>
@@ -1729,7 +1736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>42</v>
       </c>
@@ -1740,7 +1747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
         <v>43</v>
       </c>
@@ -1751,7 +1758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
         <v>44</v>
       </c>
@@ -1762,7 +1769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
         <v>45</v>
       </c>
@@ -1773,7 +1780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
         <v>46</v>
       </c>
@@ -1784,7 +1791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="s">
         <v>47</v>
       </c>
@@ -1795,7 +1802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="6" t="s">
         <v>48</v>
       </c>
@@ -1806,7 +1813,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
         <v>49</v>
       </c>
@@ -1817,7 +1824,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="6" t="s">
         <v>50</v>
       </c>
@@ -1828,7 +1835,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
         <v>51</v>
       </c>
@@ -1839,7 +1846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="6" t="s">
         <v>52</v>
       </c>
@@ -1850,7 +1857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="6" t="s">
         <v>53</v>
       </c>
@@ -1861,7 +1868,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="6" t="s">
         <v>54</v>
       </c>
@@ -1872,7 +1879,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="6" t="s">
         <v>55</v>
       </c>
@@ -1883,7 +1890,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="6" t="s">
         <v>56</v>
       </c>
@@ -1894,7 +1901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="6" t="s">
         <v>57</v>
       </c>
@@ -1905,7 +1912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="6" t="s">
         <v>58</v>
       </c>
@@ -1916,18 +1923,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="6" t="s">
         <v>59</v>
       </c>
       <c r="B49" s="7">
         <v>2012</v>
       </c>
-      <c r="C49" s="2" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
+      <c r="C49" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="6" t="s">
         <v>60</v>
       </c>
@@ -1938,7 +1945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="6" t="s">
         <v>61</v>
       </c>
@@ -1946,10 +1953,10 @@
         <v>2012</v>
       </c>
       <c r="C51" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="6" t="s">
         <v>62</v>
       </c>
@@ -1960,7 +1967,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="6" t="s">
         <v>63</v>
       </c>
@@ -1968,10 +1975,10 @@
         <v>2012</v>
       </c>
       <c r="C53" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="6" t="s">
         <v>64</v>
       </c>
@@ -1982,7 +1989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="6" t="s">
         <v>65</v>
       </c>
@@ -1990,10 +1997,10 @@
         <v>2012</v>
       </c>
       <c r="C55" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="6" t="s">
         <v>66</v>
       </c>
@@ -2001,10 +2008,10 @@
         <v>2012</v>
       </c>
       <c r="C56" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="6" t="s">
         <v>67</v>
       </c>
@@ -2012,10 +2019,10 @@
         <v>2012</v>
       </c>
       <c r="C57" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="6" t="s">
         <v>68</v>
       </c>
@@ -2023,10 +2030,10 @@
         <v>2012</v>
       </c>
       <c r="C58" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="6" t="s">
         <v>69</v>
       </c>
@@ -2034,10 +2041,10 @@
         <v>2012</v>
       </c>
       <c r="C59" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="6" t="s">
         <v>70</v>
       </c>
@@ -2045,10 +2052,10 @@
         <v>2012</v>
       </c>
       <c r="C60" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="6" t="s">
         <v>71</v>
       </c>
@@ -2056,10 +2063,10 @@
         <v>2012</v>
       </c>
       <c r="C61" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="6" t="s">
         <v>72</v>
       </c>
@@ -2070,7 +2077,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="6" t="s">
         <v>73</v>
       </c>
@@ -2081,7 +2088,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="6" t="s">
         <v>74</v>
       </c>
@@ -2089,10 +2096,10 @@
         <v>2012</v>
       </c>
       <c r="C64" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" s="6" t="s">
         <v>75</v>
       </c>
@@ -2100,10 +2107,10 @@
         <v>2012</v>
       </c>
       <c r="C65" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="6" t="s">
         <v>76</v>
       </c>
@@ -2111,10 +2118,10 @@
         <v>2012</v>
       </c>
       <c r="C66" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="6" t="s">
         <v>77</v>
       </c>
@@ -2125,7 +2132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="6" t="s">
         <v>78</v>
       </c>
@@ -2133,10 +2140,10 @@
         <v>2012</v>
       </c>
       <c r="C68" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="6" t="s">
         <v>79</v>
       </c>
@@ -2144,10 +2151,10 @@
         <v>2012</v>
       </c>
       <c r="C69" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="6" t="s">
         <v>80</v>
       </c>
@@ -2155,10 +2162,10 @@
         <v>2012</v>
       </c>
       <c r="C70" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="6" t="s">
         <v>81</v>
       </c>
@@ -2169,7 +2176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="6" t="s">
         <v>82</v>
       </c>
@@ -2177,10 +2184,10 @@
         <v>2012</v>
       </c>
       <c r="C72" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="6" t="s">
         <v>83</v>
       </c>
@@ -2188,10 +2195,10 @@
         <v>2012</v>
       </c>
       <c r="C73" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="6" t="s">
         <v>84</v>
       </c>
@@ -2199,10 +2206,10 @@
         <v>2012</v>
       </c>
       <c r="C74" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="6" t="s">
         <v>85</v>
       </c>
@@ -2210,10 +2217,10 @@
         <v>2012</v>
       </c>
       <c r="C75" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="6" t="s">
         <v>86</v>
       </c>
@@ -2224,7 +2231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="6" t="s">
         <v>87</v>
       </c>
@@ -2232,10 +2239,10 @@
         <v>2012</v>
       </c>
       <c r="C77" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" s="6" t="s">
         <v>88</v>
       </c>
@@ -2243,10 +2250,10 @@
         <v>2012</v>
       </c>
       <c r="C78" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" s="6" t="s">
         <v>89</v>
       </c>
@@ -2254,10 +2261,10 @@
         <v>2012</v>
       </c>
       <c r="C79" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" s="6" t="s">
         <v>90</v>
       </c>
@@ -2265,10 +2272,10 @@
         <v>2012</v>
       </c>
       <c r="C80" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" s="6" t="s">
         <v>91</v>
       </c>
@@ -2276,10 +2283,10 @@
         <v>2012</v>
       </c>
       <c r="C81" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" s="6" t="s">
         <v>92</v>
       </c>
@@ -2290,7 +2297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" s="6" t="s">
         <v>93</v>
       </c>
@@ -2301,7 +2308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" s="6" t="s">
         <v>94</v>
       </c>
@@ -2309,10 +2316,10 @@
         <v>2012</v>
       </c>
       <c r="C84" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" s="6" t="s">
         <v>95</v>
       </c>
@@ -2320,10 +2327,10 @@
         <v>2012</v>
       </c>
       <c r="C85" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" s="6" t="s">
         <v>96</v>
       </c>
@@ -2331,10 +2338,10 @@
         <v>2012</v>
       </c>
       <c r="C86" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" s="6" t="s">
         <v>97</v>
       </c>
@@ -2342,10 +2349,10 @@
         <v>2012</v>
       </c>
       <c r="C87" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" s="6" t="s">
         <v>98</v>
       </c>
@@ -2353,10 +2360,10 @@
         <v>2012</v>
       </c>
       <c r="C88" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" s="6" t="s">
         <v>99</v>
       </c>
@@ -2367,7 +2374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" s="6" t="s">
         <v>100</v>
       </c>
@@ -2378,7 +2385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" s="6" t="s">
         <v>101</v>
       </c>
@@ -2389,7 +2396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" s="6" t="s">
         <v>102</v>
       </c>
@@ -2397,10 +2404,10 @@
         <v>2012</v>
       </c>
       <c r="C92" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" s="6" t="s">
         <v>103</v>
       </c>
@@ -2408,10 +2415,10 @@
         <v>2012</v>
       </c>
       <c r="C93" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" s="6" t="s">
         <v>104</v>
       </c>
@@ -2419,10 +2426,10 @@
         <v>2012</v>
       </c>
       <c r="C94" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" s="6" t="s">
         <v>105</v>
       </c>
@@ -2433,7 +2440,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="96" spans="1:3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" s="6" t="s">
         <v>106</v>
       </c>
@@ -2444,7 +2451,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="97" spans="1:3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" s="6" t="s">
         <v>107</v>
       </c>
@@ -2455,7 +2462,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="98" spans="1:3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" s="6" t="s">
         <v>108</v>
       </c>
@@ -2463,10 +2470,10 @@
         <v>2012</v>
       </c>
       <c r="C98" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" s="6" t="s">
         <v>109</v>
       </c>
@@ -2474,10 +2481,10 @@
         <v>2012</v>
       </c>
       <c r="C99" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" s="6" t="s">
         <v>110</v>
       </c>
@@ -2485,10 +2492,10 @@
         <v>2012</v>
       </c>
       <c r="C100" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" s="6" t="s">
         <v>111</v>
       </c>
@@ -2496,10 +2503,10 @@
         <v>2012</v>
       </c>
       <c r="C101" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" s="6" t="s">
         <v>112</v>
       </c>
@@ -2510,7 +2517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" s="6" t="s">
         <v>113</v>
       </c>
@@ -2518,10 +2525,10 @@
         <v>2012</v>
       </c>
       <c r="C103" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" s="6" t="s">
         <v>114</v>
       </c>
@@ -2532,7 +2539,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="105" spans="1:3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" s="6" t="s">
         <v>115</v>
       </c>
@@ -2540,10 +2547,10 @@
         <v>2012</v>
       </c>
       <c r="C105" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" s="6" t="s">
         <v>116</v>
       </c>
@@ -2551,10 +2558,10 @@
         <v>2012</v>
       </c>
       <c r="C106" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" s="6" t="s">
         <v>117</v>
       </c>
@@ -2562,10 +2569,10 @@
         <v>2012</v>
       </c>
       <c r="C107" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" s="6" t="s">
         <v>118</v>
       </c>
@@ -2576,7 +2583,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="109" spans="1:3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" s="6" t="s">
         <v>119</v>
       </c>
@@ -2584,10 +2591,10 @@
         <v>2012</v>
       </c>
       <c r="C109" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" s="6" t="s">
         <v>120</v>
       </c>
@@ -2595,10 +2602,10 @@
         <v>2012</v>
       </c>
       <c r="C110" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" s="6" t="s">
         <v>121</v>
       </c>
@@ -2606,10 +2613,10 @@
         <v>2012</v>
       </c>
       <c r="C111" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" s="6" t="s">
         <v>122</v>
       </c>
@@ -2617,10 +2624,10 @@
         <v>2012</v>
       </c>
       <c r="C112" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" s="6" t="s">
         <v>123</v>
       </c>
@@ -2628,10 +2635,10 @@
         <v>2012</v>
       </c>
       <c r="C113" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" s="6" t="s">
         <v>124</v>
       </c>
@@ -2639,10 +2646,10 @@
         <v>2012</v>
       </c>
       <c r="C114" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" s="6" t="s">
         <v>125</v>
       </c>
@@ -2650,10 +2657,10 @@
         <v>2012</v>
       </c>
       <c r="C115" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" s="6" t="s">
         <v>126</v>
       </c>
@@ -2661,10 +2668,10 @@
         <v>2012</v>
       </c>
       <c r="C116" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" s="6" t="s">
         <v>127</v>
       </c>
@@ -2672,10 +2679,10 @@
         <v>2012</v>
       </c>
       <c r="C117" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" s="6" t="s">
         <v>128</v>
       </c>
@@ -2683,10 +2690,10 @@
         <v>2012</v>
       </c>
       <c r="C118" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" s="6" t="s">
         <v>129</v>
       </c>
@@ -2694,10 +2701,10 @@
         <v>2012</v>
       </c>
       <c r="C119" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" s="6" t="s">
         <v>130</v>
       </c>
@@ -2705,10 +2712,10 @@
         <v>2012</v>
       </c>
       <c r="C120" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" s="6" t="s">
         <v>131</v>
       </c>
@@ -2716,21 +2723,21 @@
         <v>2012</v>
       </c>
       <c r="C121" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" s="6" t="s">
         <v>132</v>
       </c>
       <c r="B122" s="7">
-        <v>2012</v>
+        <v>2014</v>
       </c>
       <c r="C122" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" s="6" t="s">
         <v>133</v>
       </c>
@@ -2741,7 +2748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:3">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" s="6" t="s">
         <v>134</v>
       </c>
@@ -2752,7 +2759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:3">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" s="6" t="s">
         <v>135</v>
       </c>
@@ -2763,7 +2770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:3">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" s="6" t="s">
         <v>136</v>
       </c>
@@ -2771,10 +2778,10 @@
         <v>2014</v>
       </c>
       <c r="C126" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127" s="6" t="s">
         <v>137</v>
       </c>
@@ -2782,10 +2789,10 @@
         <v>2014</v>
       </c>
       <c r="C127" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128" s="6" t="s">
         <v>138</v>
       </c>
@@ -2796,7 +2803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:3">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" s="6" t="s">
         <v>139</v>
       </c>
@@ -2807,7 +2814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:3">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" s="6" t="s">
         <v>140</v>
       </c>
@@ -2818,7 +2825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:3">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131" s="6" t="s">
         <v>141</v>
       </c>
@@ -2829,7 +2836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:3">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132" s="6" t="s">
         <v>142</v>
       </c>
@@ -2840,7 +2847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:3">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A133" s="6" t="s">
         <v>143</v>
       </c>
@@ -2848,10 +2855,10 @@
         <v>2014</v>
       </c>
       <c r="C133" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" s="6" t="s">
         <v>144</v>
       </c>
@@ -2859,10 +2866,10 @@
         <v>2014</v>
       </c>
       <c r="C134" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" s="6" t="s">
         <v>145</v>
       </c>
@@ -2873,7 +2880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:3">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" s="6" t="s">
         <v>146</v>
       </c>
@@ -2884,7 +2891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:3">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A137" s="6" t="s">
         <v>147</v>
       </c>
@@ -2895,7 +2902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:3">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138" s="6" t="s">
         <v>148</v>
       </c>
@@ -2906,7 +2913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:3">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A139" s="6" t="s">
         <v>149</v>
       </c>
@@ -2917,7 +2924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:3">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140" s="6" t="s">
         <v>150</v>
       </c>
@@ -2928,7 +2935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:3">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A141" s="6" t="s">
         <v>151</v>
       </c>
@@ -2936,10 +2943,10 @@
         <v>2014</v>
       </c>
       <c r="C141" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A142" s="6" t="s">
         <v>152</v>
       </c>
@@ -2947,10 +2954,10 @@
         <v>2014</v>
       </c>
       <c r="C142" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A143" s="6" t="s">
         <v>153</v>
       </c>
@@ -2961,7 +2968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:3">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A144" s="6" t="s">
         <v>154</v>
       </c>
@@ -2972,7 +2979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:3">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A145" s="6" t="s">
         <v>155</v>
       </c>
@@ -2983,7 +2990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:3">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A146" s="6" t="s">
         <v>156</v>
       </c>
@@ -2994,7 +3001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:3">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A147" s="6" t="s">
         <v>157</v>
       </c>
@@ -3005,7 +3012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:3">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A148" s="6" t="s">
         <v>158</v>
       </c>
@@ -3016,7 +3023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:3">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A149" s="6" t="s">
         <v>159</v>
       </c>
@@ -3027,7 +3034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:3">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A150" s="6" t="s">
         <v>160</v>
       </c>
@@ -3038,7 +3045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:3">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A151" s="6" t="s">
         <v>161</v>
       </c>
@@ -3046,10 +3053,10 @@
         <v>2014</v>
       </c>
       <c r="C151" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="152" spans="1:3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A152" s="6" t="s">
         <v>162</v>
       </c>
@@ -3057,10 +3064,10 @@
         <v>2014</v>
       </c>
       <c r="C152" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A153" s="6" t="s">
         <v>163</v>
       </c>
@@ -3071,7 +3078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:3">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A154" s="6" t="s">
         <v>164</v>
       </c>
@@ -3082,7 +3089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:3">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A155" s="6" t="s">
         <v>165</v>
       </c>
@@ -3090,10 +3097,10 @@
         <v>2014</v>
       </c>
       <c r="C155" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="156" spans="1:3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A156" s="6" t="s">
         <v>166</v>
       </c>
@@ -3101,10 +3108,10 @@
         <v>2014</v>
       </c>
       <c r="C156" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="157" spans="1:3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A157" s="6" t="s">
         <v>167</v>
       </c>
@@ -3112,10 +3119,10 @@
         <v>2014</v>
       </c>
       <c r="C157" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="158" spans="1:3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A158" s="6" t="s">
         <v>168</v>
       </c>
@@ -3123,10 +3130,10 @@
         <v>2014</v>
       </c>
       <c r="C158" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="159" spans="1:3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A159" s="6" t="s">
         <v>169</v>
       </c>
@@ -3134,10 +3141,10 @@
         <v>2014</v>
       </c>
       <c r="C159" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="160" spans="1:3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A160" s="6" t="s">
         <v>170</v>
       </c>
@@ -3148,7 +3155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:3">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A161" s="6" t="s">
         <v>171</v>
       </c>
@@ -3159,7 +3166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:3">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A162" s="6" t="s">
         <v>172</v>
       </c>
@@ -3167,10 +3174,10 @@
         <v>2014</v>
       </c>
       <c r="C162" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A163" s="6" t="s">
         <v>173</v>
       </c>
@@ -3181,7 +3188,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:3">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A164" s="6" t="s">
         <v>174</v>
       </c>
@@ -3189,10 +3196,10 @@
         <v>2014</v>
       </c>
       <c r="C164" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="165" spans="1:3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A165" s="6" t="s">
         <v>175</v>
       </c>
@@ -3200,10 +3207,10 @@
         <v>2014</v>
       </c>
       <c r="C165" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="166" spans="1:3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A166" s="6" t="s">
         <v>176</v>
       </c>
@@ -3214,7 +3221,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="167" spans="1:3">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A167" s="6" t="s">
         <v>177</v>
       </c>
@@ -3225,7 +3232,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="168" spans="1:3">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A168" s="6" t="s">
         <v>178</v>
       </c>
@@ -3236,7 +3243,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="169" spans="1:3">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A169" s="6" t="s">
         <v>179</v>
       </c>
@@ -3247,7 +3254,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="170" spans="1:3">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A170" s="6" t="s">
         <v>180</v>
       </c>
@@ -3258,7 +3265,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="171" spans="1:3">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A171" s="6" t="s">
         <v>181</v>
       </c>
@@ -3266,10 +3273,10 @@
         <v>2014</v>
       </c>
       <c r="C171" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="172" spans="1:3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A172" s="6" t="s">
         <v>182</v>
       </c>
@@ -3277,10 +3284,10 @@
         <v>2014</v>
       </c>
       <c r="C172" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="173" spans="1:3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A173" s="6" t="s">
         <v>183</v>
       </c>
@@ -3288,10 +3295,10 @@
         <v>2014</v>
       </c>
       <c r="C173" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="174" spans="1:3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A174" s="6" t="s">
         <v>184</v>
       </c>
@@ -3299,10 +3306,10 @@
         <v>2014</v>
       </c>
       <c r="C174" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="175" spans="1:3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A175" s="6" t="s">
         <v>185</v>
       </c>
@@ -3310,10 +3317,10 @@
         <v>2014</v>
       </c>
       <c r="C175" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="176" spans="1:3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A176" s="6" t="s">
         <v>186</v>
       </c>
@@ -3324,7 +3331,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="177" spans="1:3">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A177" s="6" t="s">
         <v>187</v>
       </c>
@@ -3332,10 +3339,10 @@
         <v>2014</v>
       </c>
       <c r="C177" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="178" spans="1:3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A178" s="6" t="s">
         <v>188</v>
       </c>
@@ -3343,10 +3350,10 @@
         <v>2014</v>
       </c>
       <c r="C178" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="179" spans="1:3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A179" s="6" t="s">
         <v>189</v>
       </c>
@@ -3354,10 +3361,10 @@
         <v>2014</v>
       </c>
       <c r="C179" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="180" spans="1:3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A180" s="6" t="s">
         <v>190</v>
       </c>
@@ -3365,10 +3372,10 @@
         <v>2014</v>
       </c>
       <c r="C180" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="181" spans="1:3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A181" s="6" t="s">
         <v>191</v>
       </c>
@@ -3379,7 +3386,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="182" spans="1:3">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A182" s="6" t="s">
         <v>192</v>
       </c>
@@ -3387,10 +3394,10 @@
         <v>2014</v>
       </c>
       <c r="C182" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="183" spans="1:3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A183" s="6" t="s">
         <v>193</v>
       </c>
@@ -3398,10 +3405,10 @@
         <v>2014</v>
       </c>
       <c r="C183" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="184" spans="1:3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A184" s="6" t="s">
         <v>194</v>
       </c>
@@ -3409,10 +3416,10 @@
         <v>2014</v>
       </c>
       <c r="C184" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="185" spans="1:3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A185" s="6" t="s">
         <v>195</v>
       </c>
@@ -3423,7 +3430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:3">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A186" s="6" t="s">
         <v>196</v>
       </c>
@@ -3434,7 +3441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:3">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A187" s="6" t="s">
         <v>197</v>
       </c>
@@ -3445,7 +3452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:3">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A188" s="6" t="s">
         <v>198</v>
       </c>
@@ -3456,7 +3463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:3">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A189" s="6" t="s">
         <v>199</v>
       </c>
@@ -3464,10 +3471,10 @@
         <v>2014</v>
       </c>
       <c r="C189" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="190" spans="1:3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A190" s="6" t="s">
         <v>200</v>
       </c>
@@ -3475,10 +3482,10 @@
         <v>2014</v>
       </c>
       <c r="C190" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="191" spans="1:3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A191" s="6" t="s">
         <v>201</v>
       </c>
@@ -3486,10 +3493,10 @@
         <v>2014</v>
       </c>
       <c r="C191" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="192" spans="1:3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A192" s="6" t="s">
         <v>202</v>
       </c>
@@ -3497,10 +3504,10 @@
         <v>2014</v>
       </c>
       <c r="C192" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="193" spans="1:3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A193" s="6" t="s">
         <v>203</v>
       </c>
@@ -3511,7 +3518,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="194" spans="1:3">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A194" s="6" t="s">
         <v>204</v>
       </c>
@@ -3522,7 +3529,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="195" spans="1:3">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A195" s="6" t="s">
         <v>205</v>
       </c>
@@ -3533,7 +3540,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="196" spans="1:3">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A196" s="6" t="s">
         <v>206</v>
       </c>
@@ -3544,7 +3551,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="197" spans="1:3">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A197" s="6" t="s">
         <v>207</v>
       </c>
@@ -3552,10 +3559,10 @@
         <v>2014</v>
       </c>
       <c r="C197" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="198" spans="1:3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A198" s="6" t="s">
         <v>208</v>
       </c>
@@ -3563,10 +3570,10 @@
         <v>2014</v>
       </c>
       <c r="C198" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="199" spans="1:3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A199" s="6" t="s">
         <v>209</v>
       </c>
@@ -3577,7 +3584,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="200" spans="1:3">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A200" s="6" t="s">
         <v>210</v>
       </c>
@@ -3585,10 +3592,10 @@
         <v>2014</v>
       </c>
       <c r="C200" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="201" spans="1:3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A201" s="6" t="s">
         <v>211</v>
       </c>
@@ -3596,10 +3603,10 @@
         <v>2014</v>
       </c>
       <c r="C201" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="202" spans="1:3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A202" s="6" t="s">
         <v>212</v>
       </c>
@@ -3610,7 +3617,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="203" spans="1:3">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A203" s="6" t="s">
         <v>213</v>
       </c>
@@ -3621,7 +3628,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="204" spans="1:3">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A204" s="6" t="s">
         <v>214</v>
       </c>
@@ -3629,10 +3636,10 @@
         <v>2014</v>
       </c>
       <c r="C204" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="205" spans="1:3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A205" s="6" t="s">
         <v>215</v>
       </c>
@@ -3640,10 +3647,10 @@
         <v>2014</v>
       </c>
       <c r="C205" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="206" spans="1:3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A206" s="6" t="s">
         <v>216</v>
       </c>
@@ -3654,7 +3661,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="207" spans="1:3">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A207" s="6" t="s">
         <v>217</v>
       </c>
@@ -3662,10 +3669,10 @@
         <v>2014</v>
       </c>
       <c r="C207" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="208" spans="1:3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A208" s="6" t="s">
         <v>218</v>
       </c>
@@ -3676,7 +3683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" spans="1:3">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A209" s="6" t="s">
         <v>219</v>
       </c>
@@ -3684,10 +3691,10 @@
         <v>2014</v>
       </c>
       <c r="C209" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="210" spans="1:3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A210" s="6" t="s">
         <v>220</v>
       </c>
@@ -3695,10 +3702,10 @@
         <v>2014</v>
       </c>
       <c r="C210" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="211" spans="1:3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A211" s="6" t="s">
         <v>221</v>
       </c>
@@ -3706,10 +3713,10 @@
         <v>2014</v>
       </c>
       <c r="C211" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="212" spans="1:3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A212" s="6" t="s">
         <v>222</v>
       </c>
@@ -3717,10 +3724,10 @@
         <v>2014</v>
       </c>
       <c r="C212" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="213" spans="1:3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A213" s="6" t="s">
         <v>223</v>
       </c>
@@ -3728,10 +3735,10 @@
         <v>2014</v>
       </c>
       <c r="C213" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="214" spans="1:3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A214" s="6" t="s">
         <v>224</v>
       </c>
@@ -3739,10 +3746,10 @@
         <v>2014</v>
       </c>
       <c r="C214" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="215" spans="1:3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A215" s="6" t="s">
         <v>225</v>
       </c>
@@ -3750,10 +3757,10 @@
         <v>2014</v>
       </c>
       <c r="C215" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="216" spans="1:3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A216" s="6" t="s">
         <v>226</v>
       </c>
@@ -3764,7 +3771,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="217" spans="1:3">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A217" s="6" t="s">
         <v>227</v>
       </c>
@@ -3772,10 +3779,10 @@
         <v>2014</v>
       </c>
       <c r="C217" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="218" spans="1:3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A218" s="6" t="s">
         <v>228</v>
       </c>
@@ -3783,10 +3790,10 @@
         <v>2014</v>
       </c>
       <c r="C218" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="219" spans="1:3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A219" s="6" t="s">
         <v>229</v>
       </c>
@@ -3794,10 +3801,10 @@
         <v>2014</v>
       </c>
       <c r="C219" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="220" spans="1:3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A220" s="6" t="s">
         <v>230</v>
       </c>
@@ -3808,7 +3815,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="221" spans="1:3">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A221" s="6" t="s">
         <v>231</v>
       </c>
@@ -3816,10 +3823,10 @@
         <v>2014</v>
       </c>
       <c r="C221" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="222" spans="1:3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A222" s="6" t="s">
         <v>232</v>
       </c>
@@ -3827,10 +3834,10 @@
         <v>2014</v>
       </c>
       <c r="C222" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="223" spans="1:3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A223" s="6" t="s">
         <v>233</v>
       </c>
@@ -3838,10 +3845,10 @@
         <v>2014</v>
       </c>
       <c r="C223" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="224" spans="1:3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A224" s="6" t="s">
         <v>234</v>
       </c>
@@ -3852,7 +3859,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="225" spans="1:3">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A225" s="6" t="s">
         <v>235</v>
       </c>
@@ -3860,10 +3867,10 @@
         <v>2014</v>
       </c>
       <c r="C225" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="226" spans="1:3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A226" s="6" t="s">
         <v>236</v>
       </c>
@@ -3871,10 +3878,10 @@
         <v>2014</v>
       </c>
       <c r="C226" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="227" spans="1:3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A227" s="6" t="s">
         <v>237</v>
       </c>
@@ -3882,10 +3889,10 @@
         <v>2014</v>
       </c>
       <c r="C227" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="228" spans="1:3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A228" s="6" t="s">
         <v>238</v>
       </c>
@@ -3893,10 +3900,10 @@
         <v>2014</v>
       </c>
       <c r="C228" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="229" spans="1:3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A229" s="6" t="s">
         <v>239</v>
       </c>
@@ -3907,7 +3914,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="230" spans="1:3">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A230" s="6" t="s">
         <v>240</v>
       </c>
@@ -3915,10 +3922,10 @@
         <v>2014</v>
       </c>
       <c r="C230" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="231" spans="1:3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A231" s="6" t="s">
         <v>241</v>
       </c>
@@ -3926,10 +3933,10 @@
         <v>2014</v>
       </c>
       <c r="C231" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="232" spans="1:3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A232" s="6" t="s">
         <v>242</v>
       </c>
@@ -3937,10 +3944,10 @@
         <v>2014</v>
       </c>
       <c r="C232" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="233" spans="1:3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A233" s="6" t="s">
         <v>243</v>
       </c>
@@ -3951,7 +3958,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="234" spans="1:3">
+    <row r="234" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A234" s="6" t="s">
         <v>244</v>
       </c>
@@ -3962,7 +3969,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="235" spans="1:3">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A235" s="6" t="s">
         <v>245</v>
       </c>
@@ -3970,10 +3977,10 @@
         <v>2014</v>
       </c>
       <c r="C235" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="236" spans="1:3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A236" s="6" t="s">
         <v>246</v>
       </c>
@@ -3981,10 +3988,10 @@
         <v>2014</v>
       </c>
       <c r="C236" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="237" spans="1:3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A237" s="6" t="s">
         <v>247</v>
       </c>
@@ -3992,10 +3999,10 @@
         <v>2014</v>
       </c>
       <c r="C237" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="238" spans="1:3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A238" s="6" t="s">
         <v>248</v>
       </c>
@@ -4006,7 +4013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="239" spans="1:3">
+    <row r="239" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A239" s="6" t="s">
         <v>249</v>
       </c>
@@ -4017,7 +4024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="240" spans="1:3">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A240" s="6" t="s">
         <v>250</v>
       </c>
@@ -4028,7 +4035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="241" spans="1:3">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A241" s="6" t="s">
         <v>251</v>
       </c>
@@ -4039,7 +4046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="242" spans="1:3">
+    <row r="242" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A242" s="6" t="s">
         <v>252</v>
       </c>
@@ -4047,10 +4054,10 @@
         <v>2014</v>
       </c>
       <c r="C242" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="243" spans="1:3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A243" s="6" t="s">
         <v>253</v>
       </c>
@@ -4058,10 +4065,10 @@
         <v>2014</v>
       </c>
       <c r="C243" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="244" spans="1:3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A244" s="6" t="s">
         <v>254</v>
       </c>
@@ -4072,7 +4079,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="245" spans="1:3">
+    <row r="245" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A245" s="6" t="s">
         <v>255</v>
       </c>
@@ -4083,7 +4090,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="246" spans="1:3">
+    <row r="246" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A246" s="6" t="s">
         <v>256</v>
       </c>
@@ -4094,7 +4101,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="247" spans="1:3">
+    <row r="247" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A247" s="6" t="s">
         <v>257</v>
       </c>
@@ -4102,10 +4109,10 @@
         <v>2014</v>
       </c>
       <c r="C247" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="248" spans="1:3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A248" s="6" t="s">
         <v>258</v>
       </c>
@@ -4113,10 +4120,10 @@
         <v>2014</v>
       </c>
       <c r="C248" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="249" spans="1:3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A249" s="6" t="s">
         <v>259</v>
       </c>
@@ -4127,7 +4134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:3">
+    <row r="250" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A250" s="6" t="s">
         <v>260</v>
       </c>
@@ -4135,10 +4142,10 @@
         <v>2014</v>
       </c>
       <c r="C250" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="251" spans="1:3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A251" s="6" t="s">
         <v>261</v>
       </c>
@@ -4146,10 +4153,10 @@
         <v>2014</v>
       </c>
       <c r="C251" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="252" spans="1:3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A252" s="6" t="s">
         <v>262</v>
       </c>
@@ -4157,10 +4164,10 @@
         <v>2014</v>
       </c>
       <c r="C252" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="253" spans="1:3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A253" s="6" t="s">
         <v>263</v>
       </c>
@@ -4168,10 +4175,10 @@
         <v>2014</v>
       </c>
       <c r="C253" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="254" spans="1:3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A254" s="6" t="s">
         <v>264</v>
       </c>
@@ -4179,10 +4186,10 @@
         <v>2014</v>
       </c>
       <c r="C254" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="255" spans="1:3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A255" s="6" t="s">
         <v>265</v>
       </c>
@@ -4193,7 +4200,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="256" spans="1:3">
+    <row r="256" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A256" s="6" t="s">
         <v>266</v>
       </c>
@@ -4201,10 +4208,10 @@
         <v>2014</v>
       </c>
       <c r="C256" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="257" spans="1:3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A257" s="6" t="s">
         <v>267</v>
       </c>
@@ -4212,10 +4219,10 @@
         <v>2014</v>
       </c>
       <c r="C257" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="258" spans="1:3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A258" s="6" t="s">
         <v>268</v>
       </c>
@@ -4223,10 +4230,10 @@
         <v>2014</v>
       </c>
       <c r="C258" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="259" spans="1:3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A259" s="6" t="s">
         <v>269</v>
       </c>
@@ -4234,10 +4241,10 @@
         <v>2014</v>
       </c>
       <c r="C259" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="260" spans="1:3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A260" s="6" t="s">
         <v>270</v>
       </c>
@@ -4245,10 +4252,10 @@
         <v>2014</v>
       </c>
       <c r="C260" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="261" spans="1:3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A261" s="6" t="s">
         <v>271</v>
       </c>
@@ -4256,10 +4263,10 @@
         <v>2014</v>
       </c>
       <c r="C261" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="262" spans="1:3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A262" s="6" t="s">
         <v>272</v>
       </c>
@@ -4267,10 +4274,10 @@
         <v>2014</v>
       </c>
       <c r="C262" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="263" spans="1:3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A263" s="6" t="s">
         <v>273</v>
       </c>
@@ -4278,10 +4285,10 @@
         <v>2014</v>
       </c>
       <c r="C263" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="264" spans="1:3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A264" s="6" t="s">
         <v>274</v>
       </c>
@@ -4289,10 +4296,10 @@
         <v>2014</v>
       </c>
       <c r="C264" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="265" spans="1:3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A265" s="6" t="s">
         <v>275</v>
       </c>
@@ -4303,7 +4310,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="266" spans="1:3">
+    <row r="266" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A266" s="6" t="s">
         <v>276</v>
       </c>
@@ -4314,7 +4321,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="267" spans="1:3">
+    <row r="267" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A267" s="6" t="s">
         <v>277</v>
       </c>
@@ -4325,7 +4332,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="268" spans="1:3">
+    <row r="268" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A268" s="6" t="s">
         <v>278</v>
       </c>
@@ -4333,10 +4340,10 @@
         <v>2014</v>
       </c>
       <c r="C268" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="269" spans="1:3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A269" s="6" t="s">
         <v>279</v>
       </c>
@@ -4344,10 +4351,10 @@
         <v>2014</v>
       </c>
       <c r="C269" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="270" spans="1:3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A270" s="6" t="s">
         <v>280</v>
       </c>
@@ -4358,7 +4365,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="271" spans="1:3">
+    <row r="271" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A271" s="6" t="s">
         <v>281</v>
       </c>
@@ -4366,10 +4373,10 @@
         <v>2014</v>
       </c>
       <c r="C271" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="272" spans="1:3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A272" s="6" t="s">
         <v>282</v>
       </c>
@@ -4377,10 +4384,10 @@
         <v>2014</v>
       </c>
       <c r="C272" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="273" spans="1:3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A273" s="6" t="s">
         <v>283</v>
       </c>
@@ -4388,10 +4395,10 @@
         <v>2014</v>
       </c>
       <c r="C273" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="274" spans="1:3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A274" s="6" t="s">
         <v>284</v>
       </c>
@@ -4399,10 +4406,10 @@
         <v>2014</v>
       </c>
       <c r="C274" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="275" spans="1:3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A275" s="6" t="s">
         <v>285</v>
       </c>
@@ -4413,7 +4420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="276" spans="1:3">
+    <row r="276" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A276" s="6" t="s">
         <v>286</v>
       </c>
@@ -4421,10 +4428,10 @@
         <v>2014</v>
       </c>
       <c r="C276" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="277" spans="1:3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A277" s="6" t="s">
         <v>287</v>
       </c>
@@ -4432,10 +4439,10 @@
         <v>2014</v>
       </c>
       <c r="C277" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="278" spans="1:3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A278" s="6" t="s">
         <v>288</v>
       </c>
@@ -4443,10 +4450,10 @@
         <v>2014</v>
       </c>
       <c r="C278" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="279" spans="1:3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A279" s="6" t="s">
         <v>289</v>
       </c>
@@ -4454,17 +4461,6 @@
         <v>2014</v>
       </c>
       <c r="C279" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="280" spans="1:3">
-      <c r="A280" s="6" t="s">
-        <v>290</v>
-      </c>
-      <c r="B280" s="7">
-        <v>2014</v>
-      </c>
-      <c r="C280" s="2">
         <v>0.5</v>
       </c>
     </row>
@@ -4480,20 +4476,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.8984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -4501,7 +4497,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -4509,15 +4505,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -4536,21 +4532,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>

</xml_diff>